<commit_message>
Correção de erro excel
</commit_message>
<xml_diff>
--- a/Baixa_PC/Livro1.xlsx
+++ b/Baixa_PC/Livro1.xlsx
@@ -115,7 +115,7 @@
     <x:t>12</x:t>
   </x:si>
   <x:si>
-    <x:t>l</x:t>
+    <x:t>K</x:t>
   </x:si>
   <x:si>
     <x:t>123456789</x:t>
@@ -124,7 +124,7 @@
     <x:t>eu</x:t>
   </x:si>
   <x:si>
-    <x:t>123</x:t>
+    <x:t>987654321</x:t>
   </x:si>
   <x:si>
     <x:t>Funciona ;)</x:t>
@@ -179,6 +179,9 @@
   </x:si>
   <x:si>
     <x:t>Reparado</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Avariado</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -845,7 +848,7 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="T3" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>48</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:20">

</xml_diff>